<commit_message>
A Whole Lot of Updates
A Whole Lot of Updates
</commit_message>
<xml_diff>
--- a/NC State House/HD105/Results.xlsx
+++ b/NC State House/HD105/Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echen\Documents\GitHub\QGIS-Politics\NC State House\HD105\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2139630F-18D3-4E49-9314-D1C0A0AE26EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943F3C3B-6952-4F85-84A4-81A459EE635B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HD92" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="209">
   <si>
     <t>Precinct</t>
   </si>
@@ -1654,15 +1654,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3920BBB-DE15-488B-AABE-3484E9B34F20}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1675,8 +1675,17 @@
       <c r="D1" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>75</v>
       </c>
@@ -1689,8 +1698,20 @@
       <c r="D2">
         <v>913.91255088124365</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="3">
+        <f>B2/D2</f>
+        <v>0.47478056967577481</v>
+      </c>
+      <c r="F2" s="3">
+        <f>C2/D2</f>
+        <v>0.52521943032422524</v>
+      </c>
+      <c r="G2" s="3">
+        <f>(B2-C2)/D2</f>
+        <v>-5.0438860648450393E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>73</v>
       </c>
@@ -1703,8 +1724,20 @@
       <c r="D3">
         <v>1557.4575072262778</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" s="3">
+        <f t="shared" ref="E3:E17" si="0">B3/D3</f>
+        <v>0.59288311391774828</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" ref="F3:F17" si="1">C3/D3</f>
+        <v>0.40711688608225166</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G17" si="2">(B3-C3)/D3</f>
+        <v>0.18576622783549659</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>146</v>
       </c>
@@ -1717,8 +1750,20 @@
       <c r="D4">
         <v>1249.2602423875462</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" s="3">
+        <f t="shared" si="0"/>
+        <v>0.4328816170508315</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" si="1"/>
+        <v>0.5671183829491685</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" si="2"/>
+        <v>-0.13423676589833697</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>185</v>
       </c>
@@ -1731,8 +1776,20 @@
       <c r="D5">
         <v>1879.9803340564845</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>0.54119675928111166</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" si="1"/>
+        <v>0.45880324071888834</v>
+      </c>
+      <c r="G5" s="3">
+        <f t="shared" si="2"/>
+        <v>8.2393518562223336E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>43</v>
       </c>
@@ -1745,8 +1802,20 @@
       <c r="D6">
         <v>1529.0969056917902</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
+        <v>0.4955446262379562</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="1"/>
+        <v>0.50445537376204386</v>
+      </c>
+      <c r="G6" s="3">
+        <f t="shared" si="2"/>
+        <v>-8.9107475240876154E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>53</v>
       </c>
@@ -1759,8 +1828,20 @@
       <c r="D7">
         <v>1501.9365376425942</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>0.4354831792743325</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" si="1"/>
+        <v>0.56451682072566756</v>
+      </c>
+      <c r="G7" s="3">
+        <f t="shared" si="2"/>
+        <v>-0.12903364145133506</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>194</v>
       </c>
@@ -1773,8 +1854,20 @@
       <c r="D8">
         <v>2738.3999417124237</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
+        <v>0.45194254586103905</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="1"/>
+        <v>0.5480574541389609</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" si="2"/>
+        <v>-9.6114908277921879E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -1787,8 +1880,20 @@
       <c r="D9">
         <v>1248.1367552997935</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>0.47351583174990514</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="1"/>
+        <v>0.52648416825009492</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" si="2"/>
+        <v>-5.2968336500189811E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>128</v>
       </c>
@@ -1801,8 +1906,20 @@
       <c r="D10">
         <v>3483.569908117508</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
+        <v>0.46417948557400379</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="1"/>
+        <v>0.53582051442599621</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" si="2"/>
+        <v>-7.1641028851992472E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>186</v>
       </c>
@@ -1815,8 +1932,20 @@
       <c r="D11">
         <v>2101.1531970023771</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>0.53661929762284577</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="1"/>
+        <v>0.46338070237715429</v>
+      </c>
+      <c r="G11" s="3">
+        <f t="shared" si="2"/>
+        <v>7.3238595245691512E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>161</v>
       </c>
@@ -1829,8 +1958,20 @@
       <c r="D12">
         <v>3224.469123873243</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>0.53130859907999206</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="1"/>
+        <v>0.46869140092000788</v>
+      </c>
+      <c r="G12" s="3">
+        <f t="shared" si="2"/>
+        <v>6.2617198159984205E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>133</v>
       </c>
@@ -1843,8 +1984,20 @@
       <c r="D13">
         <v>2248.0523850380146</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13" s="3">
+        <f t="shared" si="0"/>
+        <v>0.52960284437978089</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="1"/>
+        <v>0.47039715562021905</v>
+      </c>
+      <c r="G13" s="3">
+        <f t="shared" si="2"/>
+        <v>5.9205688759561857E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>113</v>
       </c>
@@ -1857,8 +2010,20 @@
       <c r="D14">
         <v>6075.3608667597091</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14" s="3">
+        <f t="shared" si="0"/>
+        <v>0.61341079301457757</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="1"/>
+        <v>0.38658920698542232</v>
+      </c>
+      <c r="G14" s="3">
+        <f t="shared" si="2"/>
+        <v>0.22682158602915531</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>85</v>
       </c>
@@ -1871,8 +2036,20 @@
       <c r="D15">
         <v>2212.38479891833</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15" s="3">
+        <f t="shared" si="0"/>
+        <v>0.56181146040506524</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="1"/>
+        <v>0.4381885395949347</v>
+      </c>
+      <c r="G15" s="3">
+        <f t="shared" si="2"/>
+        <v>0.12362292081013058</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>144</v>
       </c>
@@ -1884,6 +2061,47 @@
       </c>
       <c r="D16">
         <v>3151.8289453926645</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="0"/>
+        <v>0.50388068956324439</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="1"/>
+        <v>0.49611931043675556</v>
+      </c>
+      <c r="G16" s="3">
+        <f t="shared" si="2"/>
+        <v>7.7613791264888477E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B17">
+        <f>SUM(B2:B16)</f>
+        <v>18362</v>
+      </c>
+      <c r="C17">
+        <f>SUM(C2:C16)</f>
+        <v>16753</v>
+      </c>
+      <c r="D17">
+        <f>SUM(D2:D16)</f>
+        <v>35115.000000000007</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="0"/>
+        <v>0.5229104371351273</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" si="1"/>
+        <v>0.47708956286487247</v>
+      </c>
+      <c r="G17" s="3">
+        <f t="shared" si="2"/>
+        <v>4.5820874270254865E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1898,7 +2116,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0F9A052-6D50-4507-9C0B-D7FB1970D0EE}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>

</xml_diff>